<commit_message>
Deploying to gh-pages from @ Healthedata1/test-stuff@1678d7a060325814e3a82fe06f614b5886b7a6f7 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-pmo-servicerequest.xlsx
+++ b/StructureDefinition-us-core-pmo-servicerequest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1959" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1959" uniqueCount="470">
   <si>
     <t>Property</t>
   </si>
@@ -740,10 +740,15 @@
     <t>us-core-pmo</t>
   </si>
   <si>
+    <t xml:space="preserve">100821-8 (National POLST Form: A Portable Medical Order panel) | 100822-6 (Cardiopulmonary resuscitation orders) | 100823-4 (Initial portable medical treatment orders) | 100824-2 (Additional portable medical orders or instructions) | 100825-9 (Medically assisted nutrition orders) | 100970-3 (Portable medical order completion information) | 100826-7 (Portable medical order &amp;or advance directive review) | 100827-5 (Portable medical order discussion participants) | 100828-3 (Portable medical order administrative information)
+</t>
+  </si>
+  <si>
     <t>extensible</t>
   </si>
   <si>
-    <t>[Portable Medical Order panel codes](https://loinc.org/100821-8)</t>
+    <t xml:space="preserve">[Portable Medical Order panel codes](https://loinc.org/100821-8)
+</t>
   </si>
   <si>
     <t>http://hl7.org/fhir/us/core/ValueSet/us-core-pmo-servicerequest-category</t>
@@ -4111,7 +4116,7 @@
         <v>218</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>219</v>
+        <v>232</v>
       </c>
       <c r="M20" t="s" s="2">
         <v>220</v>
@@ -4145,13 +4150,13 @@
         <v>81</v>
       </c>
       <c r="X20" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="Y20" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="Z20" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="AA20" t="s" s="2">
         <v>81</v>
@@ -4201,10 +4206,10 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -4230,10 +4235,10 @@
         <v>110</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
@@ -4241,7 +4246,7 @@
         <v>81</v>
       </c>
       <c r="Q21" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="R21" t="s" s="2">
         <v>81</v>
@@ -4265,10 +4270,10 @@
         <v>199</v>
       </c>
       <c r="Y21" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="Z21" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AA21" t="s" s="2">
         <v>81</v>
@@ -4286,7 +4291,7 @@
         <v>81</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>79</v>
@@ -4301,16 +4306,16 @@
         <v>102</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>81</v>
@@ -4318,10 +4323,10 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -4344,70 +4349,70 @@
         <v>91</v>
       </c>
       <c r="K22" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="L22" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="M22" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="N22" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="O22" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="P22" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="Q22" t="s" s="2">
+        <v>252</v>
+      </c>
+      <c r="R22" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="S22" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="T22" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="U22" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="V22" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="W22" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="X22" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="Y22" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="Z22" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AA22" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AB22" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AC22" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AD22" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AE22" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AF22" t="s" s="2">
         <v>246</v>
-      </c>
-      <c r="L22" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="M22" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="N22" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="O22" t="s" s="2">
-        <v>250</v>
-      </c>
-      <c r="P22" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="Q22" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="R22" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="S22" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="T22" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="U22" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="V22" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="W22" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="X22" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="Y22" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="Z22" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AA22" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AB22" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AC22" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AD22" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AE22" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AF22" t="s" s="2">
-        <v>245</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>79</v>
@@ -4422,13 +4427,13 @@
         <v>102</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AL22" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN22" t="s" s="2">
         <v>81</v>
@@ -4439,14 +4444,14 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" t="s" s="2">
@@ -4468,13 +4473,13 @@
         <v>218</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" t="s" s="2">
@@ -4500,13 +4505,13 @@
         <v>81</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="Z23" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AA23" t="s" s="2">
         <v>81</v>
@@ -4524,7 +4529,7 @@
         <v>81</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>79</v>
@@ -4539,27 +4544,27 @@
         <v>102</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AO23" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -4582,13 +4587,13 @@
         <v>81</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -4639,7 +4644,7 @@
         <v>81</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>79</v>
@@ -4660,7 +4665,7 @@
         <v>81</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AN24" t="s" s="2">
         <v>81</v>
@@ -4671,10 +4676,10 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -4703,7 +4708,7 @@
         <v>137</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="N25" t="s" s="2">
         <v>139</v>
@@ -4744,10 +4749,10 @@
         <v>81</v>
       </c>
       <c r="AB25" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AC25" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="AD25" t="s" s="2">
         <v>81</v>
@@ -4756,7 +4761,7 @@
         <v>227</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>79</v>
@@ -4777,7 +4782,7 @@
         <v>81</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>81</v>
@@ -4788,10 +4793,10 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -4814,19 +4819,19 @@
         <v>91</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="O26" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="P26" t="s" s="2">
         <v>81</v>
@@ -4875,7 +4880,7 @@
         <v>81</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>79</v>
@@ -4893,10 +4898,10 @@
         <v>81</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>81</v>
@@ -4907,10 +4912,10 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4933,19 +4938,19 @@
         <v>91</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O27" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="P27" t="s" s="2">
         <v>81</v>
@@ -4994,7 +4999,7 @@
         <v>81</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>79</v>
@@ -5012,10 +5017,10 @@
         <v>81</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>81</v>
@@ -5026,14 +5031,14 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" t="s" s="2">
@@ -5055,13 +5060,13 @@
         <v>218</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" t="s" s="2">
@@ -5090,10 +5095,10 @@
         <v>223</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="Z28" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="AA28" t="s" s="2">
         <v>81</v>
@@ -5111,7 +5116,7 @@
         <v>81</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>79</v>
@@ -5120,7 +5125,7 @@
         <v>80</v>
       </c>
       <c r="AI28" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="AJ28" t="s" s="2">
         <v>102</v>
@@ -5129,24 +5134,24 @@
         <v>81</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO28" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -5169,13 +5174,13 @@
         <v>81</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -5226,7 +5231,7 @@
         <v>81</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>79</v>
@@ -5247,7 +5252,7 @@
         <v>81</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>81</v>
@@ -5258,10 +5263,10 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5290,7 +5295,7 @@
         <v>137</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="N30" t="s" s="2">
         <v>139</v>
@@ -5331,10 +5336,10 @@
         <v>81</v>
       </c>
       <c r="AB30" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AC30" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="AD30" t="s" s="2">
         <v>81</v>
@@ -5343,7 +5348,7 @@
         <v>227</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>79</v>
@@ -5364,7 +5369,7 @@
         <v>81</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>81</v>
@@ -5375,10 +5380,10 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5401,19 +5406,19 @@
         <v>91</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="O31" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="P31" t="s" s="2">
         <v>81</v>
@@ -5462,7 +5467,7 @@
         <v>81</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>79</v>
@@ -5480,10 +5485,10 @@
         <v>81</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>81</v>
@@ -5494,10 +5499,10 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5520,19 +5525,19 @@
         <v>91</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O32" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="P32" t="s" s="2">
         <v>81</v>
@@ -5581,7 +5586,7 @@
         <v>81</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>79</v>
@@ -5599,10 +5604,10 @@
         <v>81</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>81</v>
@@ -5613,10 +5618,10 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5639,17 +5644,17 @@
         <v>91</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="P33" t="s" s="2">
         <v>81</v>
@@ -5698,7 +5703,7 @@
         <v>81</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>79</v>
@@ -5716,10 +5721,10 @@
         <v>81</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>81</v>
@@ -5730,10 +5735,10 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5756,13 +5761,13 @@
         <v>91</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -5813,7 +5818,7 @@
         <v>81</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>90</v>
@@ -5828,31 +5833,31 @@
         <v>102</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="AN34" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="AO34" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" t="s" s="2">
@@ -5871,13 +5876,13 @@
         <v>91</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
@@ -5928,7 +5933,7 @@
         <v>81</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>79</v>
@@ -5943,31 +5948,31 @@
         <v>102</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="AN35" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="AO35" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" t="s" s="2">
@@ -5986,13 +5991,13 @@
         <v>91</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -6043,7 +6048,7 @@
         <v>81</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>79</v>
@@ -6058,27 +6063,27 @@
         <v>102</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="AO36" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -6101,13 +6106,13 @@
         <v>91</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -6137,10 +6142,10 @@
         <v>223</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="Z37" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="AA37" t="s" s="2">
         <v>81</v>
@@ -6158,7 +6163,7 @@
         <v>81</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>79</v>
@@ -6179,25 +6184,25 @@
         <v>81</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO37" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" t="s" s="2">
@@ -6216,13 +6221,13 @@
         <v>91</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
@@ -6273,7 +6278,7 @@
         <v>81</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>79</v>
@@ -6288,31 +6293,31 @@
         <v>102</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AO38" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" t="s" s="2">
@@ -6331,16 +6336,16 @@
         <v>91</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="O39" s="2"/>
       <c r="P39" t="s" s="2">
@@ -6390,7 +6395,7 @@
         <v>81</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>79</v>
@@ -6405,31 +6410,31 @@
         <v>102</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AN39" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="AO39" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" t="s" s="2">
@@ -6451,13 +6456,13 @@
         <v>218</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="O40" s="2"/>
       <c r="P40" t="s" s="2">
@@ -6486,10 +6491,10 @@
         <v>223</v>
       </c>
       <c r="Y40" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="Z40" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="AA40" t="s" s="2">
         <v>81</v>
@@ -6507,7 +6512,7 @@
         <v>81</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>79</v>
@@ -6522,16 +6527,16 @@
         <v>102</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AN40" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="AO40" t="s" s="2">
         <v>81</v>
@@ -6539,14 +6544,14 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" t="s" s="2">
@@ -6565,16 +6570,16 @@
         <v>91</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="O41" s="2"/>
       <c r="P41" t="s" s="2">
@@ -6624,7 +6629,7 @@
         <v>81</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>79</v>
@@ -6639,16 +6644,16 @@
         <v>102</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="AN41" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="AO41" t="s" s="2">
         <v>81</v>
@@ -6656,10 +6661,10 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6685,10 +6690,10 @@
         <v>218</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
@@ -6718,10 +6723,10 @@
         <v>223</v>
       </c>
       <c r="Y42" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="Z42" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="AA42" t="s" s="2">
         <v>81</v>
@@ -6739,7 +6744,7 @@
         <v>81</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>79</v>
@@ -6760,10 +6765,10 @@
         <v>81</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="AN42" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="AO42" t="s" s="2">
         <v>81</v>
@@ -6771,10 +6776,10 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6797,13 +6802,13 @@
         <v>91</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
@@ -6854,7 +6859,7 @@
         <v>81</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>79</v>
@@ -6875,10 +6880,10 @@
         <v>81</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="AN43" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="AO43" t="s" s="2">
         <v>81</v>
@@ -6886,10 +6891,10 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6915,13 +6920,13 @@
         <v>218</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="N44" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="O44" s="2"/>
       <c r="P44" t="s" s="2">
@@ -6947,11 +6952,11 @@
         <v>81</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="Y44" s="2"/>
       <c r="Z44" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="AA44" t="s" s="2">
         <v>81</v>
@@ -6969,7 +6974,7 @@
         <v>81</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>79</v>
@@ -6984,16 +6989,16 @@
         <v>102</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="AN44" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="AO44" t="s" s="2">
         <v>81</v>
@@ -7001,10 +7006,10 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -7027,16 +7032,16 @@
         <v>91</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="N45" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="O45" s="2"/>
       <c r="P45" t="s" s="2">
@@ -7086,7 +7091,7 @@
         <v>81</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>79</v>
@@ -7101,16 +7106,16 @@
         <v>102</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="AN45" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="AO45" t="s" s="2">
         <v>81</v>
@@ -7118,10 +7123,10 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -7144,13 +7149,13 @@
         <v>81</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
@@ -7201,7 +7206,7 @@
         <v>81</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>79</v>
@@ -7216,13 +7221,13 @@
         <v>102</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>81</v>
@@ -7233,14 +7238,14 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" t="s" s="2">
@@ -7259,16 +7264,16 @@
         <v>81</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="O47" s="2"/>
       <c r="P47" t="s" s="2">
@@ -7318,7 +7323,7 @@
         <v>81</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>79</v>
@@ -7333,13 +7338,13 @@
         <v>102</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>81</v>
@@ -7350,10 +7355,10 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7376,16 +7381,16 @@
         <v>91</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="O48" s="2"/>
       <c r="P48" t="s" s="2">
@@ -7435,7 +7440,7 @@
         <v>81</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>79</v>
@@ -7453,10 +7458,10 @@
         <v>81</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>81</v>
@@ -7467,14 +7472,14 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" t="s" s="2">
@@ -7496,16 +7501,16 @@
         <v>218</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="O49" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="P49" t="s" s="2">
         <v>81</v>
@@ -7533,10 +7538,10 @@
         <v>223</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="Z49" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AA49" t="s" s="2">
         <v>81</v>
@@ -7554,7 +7559,7 @@
         <v>81</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>79</v>
@@ -7572,24 +7577,24 @@
         <v>81</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO49" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -7612,13 +7617,13 @@
         <v>81</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="L50" t="s" s="2">
         <v>50</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
@@ -7669,7 +7674,7 @@
         <v>81</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>79</v>
@@ -7684,27 +7689,27 @@
         <v>102</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7727,13 +7732,13 @@
         <v>91</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
@@ -7784,7 +7789,7 @@
         <v>81</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>79</v>
@@ -7802,10 +7807,10 @@
         <v>81</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>81</v>
@@ -7816,10 +7821,10 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -7842,16 +7847,16 @@
         <v>81</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="O52" s="2"/>
       <c r="P52" t="s" s="2">
@@ -7901,7 +7906,7 @@
         <v>81</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>79</v>
@@ -7916,13 +7921,13 @@
         <v>102</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="AL52" t="s" s="2">
         <v>133</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>81</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ Healthedata1/test-stuff@055a499157fec3befa9e5d9eed30425a23554571 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-pmo-servicerequest.xlsx
+++ b/StructureDefinition-us-core-pmo-servicerequest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1959" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1959" uniqueCount="469">
   <si>
     <t>Property</t>
   </si>
@@ -666,16 +666,13 @@
     <t>ServiceRequest.intent</t>
   </si>
   <si>
-    <t>proposal | plan | directive | order | original-order | reflex-order | filler-order | instance-order | option</t>
+    <t>Note: To allow for the resource life cycle, no constraint on intent, use "directive" in PMO document</t>
   </si>
   <si>
     <t>Whether the request is a proposal, plan, an original order or a reflex order.</t>
   </si>
   <si>
     <t>This element is labeled as a modifier because the intent alters when and how the resource is actually applicable.</t>
-  </si>
-  <si>
-    <t>directive</t>
   </si>
   <si>
     <t>The kind of service request.</t>
@@ -740,8 +737,7 @@
     <t>us-core-pmo</t>
   </si>
   <si>
-    <t xml:space="preserve">100821-8 (National POLST Form: A Portable Medical Order panel) | 100822-6 (Cardiopulmonary resuscitation orders) | 100823-4 (Initial portable medical treatment orders) | 100824-2 (Additional portable medical orders or instructions) | 100825-9 (Medically assisted nutrition orders) | 100970-3 (Portable medical order completion information) | 100826-7 (Portable medical order &amp;or advance directive review) | 100827-5 (Portable medical order discussion participants) | 100828-3 (Portable medical order administrative information)
-</t>
+    <t>Multiple portable medical order categories vs a single "PMO" category (2 vs 3 level code heirarchy)?</t>
   </si>
   <si>
     <t>extensible</t>
@@ -751,7 +747,7 @@
 </t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/ValueSet/us-core-pmo-servicerequest-category</t>
+    <t>http://hl7.org/fhir/us/core/ValueSet/us-core-portable-medical-orders</t>
   </si>
   <si>
     <t>ServiceRequest.priority</t>
@@ -1002,11 +998,11 @@
     <t>ServiceRequest.subject</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient|Group|http://hl7.org/fhir/us/core/StructureDefinition/us-core-location|Device)
+    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient)
 </t>
   </si>
   <si>
-    <t>Individual or Entity the service is ordered for</t>
+    <t>limited to Patient</t>
   </si>
   <si>
     <t>On whom or what the service is to be performed. This is usually a human patient, but can also be requested on animals, groups of humans or animals, devices such as dialysis machines, or even locations (typically for environmental scans).</t>
@@ -1038,7 +1034,7 @@
 </t>
   </si>
   <si>
-    <t>Encounter in which the request was created</t>
+    <t>**NOT USED WHEN PART OF A PMO DOCUMENT**</t>
   </si>
   <si>
     <t>An encounter that provides additional information about the healthcare context in which this request is made.</t>
@@ -1070,7 +1066,7 @@
 dateTimeTiming</t>
   </si>
   <si>
-    <t>When service should occur</t>
+    <t>Often just a start date</t>
   </si>
   <si>
     <t>The date/time at which the requested service should occur.</t>
@@ -1127,7 +1123,7 @@
 </t>
   </si>
   <si>
-    <t>Date request signed</t>
+    <t>Date Order signed vs date of PMO document - same if part of PMO document</t>
   </si>
   <si>
     <t>When the request transitioned to being actionable.</t>
@@ -1155,11 +1151,11 @@
 orderer</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner|http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization|http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient|PractitionerRole|http://hl7.org/fhir/us/core/StructureDefinition/us-core-relatedperson|Device)
+    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner|http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization|PractitionerRole)
 </t>
   </si>
   <si>
-    <t>Who/what is requesting service</t>
+    <t>Authored only by Practitioner</t>
   </si>
   <si>
     <t>The individual who initiated the request and has responsibility for its activation.</t>
@@ -1824,7 +1820,7 @@
     <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="235.17578125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="127.171875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1839,7 +1835,7 @@
     <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="108.3203125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="58.3984375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="58.125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="36.0390625" customWidth="true" bestFit="true"/>
@@ -3894,7 +3890,7 @@
       </c>
       <c r="Q18" s="2"/>
       <c r="R18" t="s" s="2">
-        <v>211</v>
+        <v>81</v>
       </c>
       <c r="S18" t="s" s="2">
         <v>81</v>
@@ -3915,10 +3911,10 @@
         <v>199</v>
       </c>
       <c r="Y18" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="Z18" t="s" s="2">
         <v>212</v>
-      </c>
-      <c r="Z18" t="s" s="2">
-        <v>213</v>
       </c>
       <c r="AA18" t="s" s="2">
         <v>81</v>
@@ -3951,16 +3947,16 @@
         <v>102</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AL18" t="s" s="2">
         <v>133</v>
       </c>
       <c r="AM18" t="s" s="2">
+        <v>214</v>
+      </c>
+      <c r="AN18" t="s" s="2">
         <v>215</v>
-      </c>
-      <c r="AN18" t="s" s="2">
-        <v>216</v>
       </c>
       <c r="AO18" t="s" s="2">
         <v>81</v>
@@ -3968,10 +3964,10 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -3994,19 +3990,19 @@
         <v>91</v>
       </c>
       <c r="K19" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="L19" t="s" s="2">
         <v>218</v>
       </c>
-      <c r="L19" t="s" s="2">
+      <c r="M19" t="s" s="2">
         <v>219</v>
       </c>
-      <c r="M19" t="s" s="2">
+      <c r="N19" t="s" s="2">
         <v>220</v>
       </c>
-      <c r="N19" t="s" s="2">
+      <c r="O19" t="s" s="2">
         <v>221</v>
-      </c>
-      <c r="O19" t="s" s="2">
-        <v>222</v>
       </c>
       <c r="P19" t="s" s="2">
         <v>81</v>
@@ -4031,29 +4027,29 @@
         <v>81</v>
       </c>
       <c r="X19" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="Y19" t="s" s="2">
         <v>223</v>
       </c>
-      <c r="Y19" t="s" s="2">
+      <c r="Z19" t="s" s="2">
         <v>224</v>
       </c>
-      <c r="Z19" t="s" s="2">
+      <c r="AA19" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AB19" t="s" s="2">
         <v>225</v>
-      </c>
-      <c r="AA19" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AB19" t="s" s="2">
-        <v>226</v>
       </c>
       <c r="AC19" s="2"/>
       <c r="AD19" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>79</v>
@@ -4071,13 +4067,13 @@
         <v>81</v>
       </c>
       <c r="AL19" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AM19" t="s" s="2">
         <v>228</v>
       </c>
-      <c r="AM19" t="s" s="2">
-        <v>229</v>
-      </c>
       <c r="AN19" t="s" s="2">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>81</v>
@@ -4085,13 +4081,13 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
+        <v>229</v>
+      </c>
+      <c r="B20" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="C20" t="s" s="2">
         <v>230</v>
-      </c>
-      <c r="B20" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="C20" t="s" s="2">
-        <v>231</v>
       </c>
       <c r="D20" t="s" s="2">
         <v>81</v>
@@ -4113,19 +4109,19 @@
         <v>91</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M20" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="N20" t="s" s="2">
         <v>220</v>
       </c>
-      <c r="N20" t="s" s="2">
+      <c r="O20" t="s" s="2">
         <v>221</v>
-      </c>
-      <c r="O20" t="s" s="2">
-        <v>222</v>
       </c>
       <c r="P20" t="s" s="2">
         <v>81</v>
@@ -4150,14 +4146,14 @@
         <v>81</v>
       </c>
       <c r="X20" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="Y20" t="s" s="2">
         <v>233</v>
       </c>
-      <c r="Y20" t="s" s="2">
+      <c r="Z20" t="s" s="2">
         <v>234</v>
       </c>
-      <c r="Z20" t="s" s="2">
-        <v>235</v>
-      </c>
       <c r="AA20" t="s" s="2">
         <v>81</v>
       </c>
@@ -4174,7 +4170,7 @@
         <v>81</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>79</v>
@@ -4192,13 +4188,13 @@
         <v>81</v>
       </c>
       <c r="AL20" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AM20" t="s" s="2">
         <v>228</v>
       </c>
-      <c r="AM20" t="s" s="2">
-        <v>229</v>
-      </c>
       <c r="AN20" t="s" s="2">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AO20" t="s" s="2">
         <v>81</v>
@@ -4206,10 +4202,10 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -4235,10 +4231,10 @@
         <v>110</v>
       </c>
       <c r="L21" t="s" s="2">
+        <v>236</v>
+      </c>
+      <c r="M21" t="s" s="2">
         <v>237</v>
-      </c>
-      <c r="M21" t="s" s="2">
-        <v>238</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
@@ -4246,7 +4242,7 @@
         <v>81</v>
       </c>
       <c r="Q21" t="s" s="2">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="R21" t="s" s="2">
         <v>81</v>
@@ -4270,11 +4266,11 @@
         <v>199</v>
       </c>
       <c r="Y21" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="Z21" t="s" s="2">
         <v>240</v>
       </c>
-      <c r="Z21" t="s" s="2">
-        <v>241</v>
-      </c>
       <c r="AA21" t="s" s="2">
         <v>81</v>
       </c>
@@ -4291,7 +4287,7 @@
         <v>81</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>79</v>
@@ -4306,16 +4302,16 @@
         <v>102</v>
       </c>
       <c r="AK21" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="AL21" t="s" s="2">
         <v>242</v>
       </c>
-      <c r="AL21" t="s" s="2">
+      <c r="AM21" t="s" s="2">
         <v>243</v>
       </c>
-      <c r="AM21" t="s" s="2">
+      <c r="AN21" t="s" s="2">
         <v>244</v>
-      </c>
-      <c r="AN21" t="s" s="2">
-        <v>245</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>81</v>
@@ -4323,10 +4319,10 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -4349,26 +4345,26 @@
         <v>91</v>
       </c>
       <c r="K22" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="L22" t="s" s="2">
         <v>247</v>
       </c>
-      <c r="L22" t="s" s="2">
+      <c r="M22" t="s" s="2">
         <v>248</v>
       </c>
-      <c r="M22" t="s" s="2">
+      <c r="N22" t="s" s="2">
         <v>249</v>
       </c>
-      <c r="N22" t="s" s="2">
+      <c r="O22" t="s" s="2">
         <v>250</v>
       </c>
-      <c r="O22" t="s" s="2">
+      <c r="P22" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="Q22" t="s" s="2">
         <v>251</v>
       </c>
-      <c r="P22" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="Q22" t="s" s="2">
-        <v>252</v>
-      </c>
       <c r="R22" t="s" s="2">
         <v>81</v>
       </c>
@@ -4412,7 +4408,7 @@
         <v>81</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>79</v>
@@ -4427,13 +4423,13 @@
         <v>102</v>
       </c>
       <c r="AK22" t="s" s="2">
+        <v>252</v>
+      </c>
+      <c r="AL22" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AM22" t="s" s="2">
         <v>253</v>
-      </c>
-      <c r="AL22" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AM22" t="s" s="2">
-        <v>254</v>
       </c>
       <c r="AN22" t="s" s="2">
         <v>81</v>
@@ -4444,14 +4440,14 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" t="s" s="2">
@@ -4470,16 +4466,16 @@
         <v>91</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L23" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="M23" t="s" s="2">
         <v>257</v>
       </c>
-      <c r="M23" t="s" s="2">
+      <c r="N23" t="s" s="2">
         <v>258</v>
-      </c>
-      <c r="N23" t="s" s="2">
-        <v>259</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" t="s" s="2">
@@ -4505,14 +4501,14 @@
         <v>81</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Y23" t="s" s="2">
+        <v>259</v>
+      </c>
+      <c r="Z23" t="s" s="2">
         <v>260</v>
       </c>
-      <c r="Z23" t="s" s="2">
-        <v>261</v>
-      </c>
       <c r="AA23" t="s" s="2">
         <v>81</v>
       </c>
@@ -4529,7 +4525,7 @@
         <v>81</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>79</v>
@@ -4544,27 +4540,27 @@
         <v>102</v>
       </c>
       <c r="AK23" t="s" s="2">
+        <v>261</v>
+      </c>
+      <c r="AL23" t="s" s="2">
         <v>262</v>
       </c>
-      <c r="AL23" t="s" s="2">
+      <c r="AM23" t="s" s="2">
         <v>263</v>
       </c>
-      <c r="AM23" t="s" s="2">
+      <c r="AN23" t="s" s="2">
         <v>264</v>
       </c>
-      <c r="AN23" t="s" s="2">
+      <c r="AO23" t="s" s="2">
         <v>265</v>
-      </c>
-      <c r="AO23" t="s" s="2">
-        <v>266</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -4587,13 +4583,13 @@
         <v>81</v>
       </c>
       <c r="K24" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="L24" t="s" s="2">
         <v>268</v>
       </c>
-      <c r="L24" t="s" s="2">
+      <c r="M24" t="s" s="2">
         <v>269</v>
-      </c>
-      <c r="M24" t="s" s="2">
-        <v>270</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -4644,7 +4640,7 @@
         <v>81</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>79</v>
@@ -4665,7 +4661,7 @@
         <v>81</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AN24" t="s" s="2">
         <v>81</v>
@@ -4676,10 +4672,10 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -4708,7 +4704,7 @@
         <v>137</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N25" t="s" s="2">
         <v>139</v>
@@ -4749,19 +4745,19 @@
         <v>81</v>
       </c>
       <c r="AB25" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="AC25" t="s" s="2">
         <v>275</v>
       </c>
-      <c r="AC25" t="s" s="2">
+      <c r="AD25" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AE25" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="AF25" t="s" s="2">
         <v>276</v>
-      </c>
-      <c r="AD25" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AE25" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="AF25" t="s" s="2">
-        <v>277</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>79</v>
@@ -4782,7 +4778,7 @@
         <v>81</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>81</v>
@@ -4793,10 +4789,10 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -4819,19 +4815,19 @@
         <v>91</v>
       </c>
       <c r="K26" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="L26" t="s" s="2">
         <v>279</v>
       </c>
-      <c r="L26" t="s" s="2">
+      <c r="M26" t="s" s="2">
         <v>280</v>
       </c>
-      <c r="M26" t="s" s="2">
+      <c r="N26" t="s" s="2">
         <v>281</v>
       </c>
-      <c r="N26" t="s" s="2">
+      <c r="O26" t="s" s="2">
         <v>282</v>
-      </c>
-      <c r="O26" t="s" s="2">
-        <v>283</v>
       </c>
       <c r="P26" t="s" s="2">
         <v>81</v>
@@ -4880,7 +4876,7 @@
         <v>81</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>79</v>
@@ -4898,10 +4894,10 @@
         <v>81</v>
       </c>
       <c r="AL26" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="AM26" t="s" s="2">
         <v>285</v>
-      </c>
-      <c r="AM26" t="s" s="2">
-        <v>286</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>81</v>
@@ -4912,10 +4908,10 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4938,19 +4934,19 @@
         <v>91</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L27" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="M27" t="s" s="2">
         <v>288</v>
       </c>
-      <c r="M27" t="s" s="2">
+      <c r="N27" t="s" s="2">
         <v>289</v>
       </c>
-      <c r="N27" t="s" s="2">
+      <c r="O27" t="s" s="2">
         <v>290</v>
-      </c>
-      <c r="O27" t="s" s="2">
-        <v>291</v>
       </c>
       <c r="P27" t="s" s="2">
         <v>81</v>
@@ -4999,7 +4995,7 @@
         <v>81</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>79</v>
@@ -5017,10 +5013,10 @@
         <v>81</v>
       </c>
       <c r="AL27" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="AM27" t="s" s="2">
         <v>293</v>
-      </c>
-      <c r="AM27" t="s" s="2">
-        <v>294</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>81</v>
@@ -5031,14 +5027,14 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" t="s" s="2">
@@ -5057,16 +5053,16 @@
         <v>91</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L28" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="M28" t="s" s="2">
         <v>297</v>
       </c>
-      <c r="M28" t="s" s="2">
+      <c r="N28" t="s" s="2">
         <v>298</v>
-      </c>
-      <c r="N28" t="s" s="2">
-        <v>299</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" t="s" s="2">
@@ -5092,14 +5088,14 @@
         <v>81</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y28" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="Z28" t="s" s="2">
         <v>300</v>
       </c>
-      <c r="Z28" t="s" s="2">
-        <v>301</v>
-      </c>
       <c r="AA28" t="s" s="2">
         <v>81</v>
       </c>
@@ -5116,7 +5112,7 @@
         <v>81</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>79</v>
@@ -5125,7 +5121,7 @@
         <v>80</v>
       </c>
       <c r="AI28" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AJ28" t="s" s="2">
         <v>102</v>
@@ -5134,24 +5130,24 @@
         <v>81</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO28" t="s" s="2">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -5174,13 +5170,13 @@
         <v>81</v>
       </c>
       <c r="K29" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="L29" t="s" s="2">
         <v>268</v>
       </c>
-      <c r="L29" t="s" s="2">
+      <c r="M29" t="s" s="2">
         <v>269</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>270</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -5231,7 +5227,7 @@
         <v>81</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>79</v>
@@ -5252,7 +5248,7 @@
         <v>81</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>81</v>
@@ -5263,10 +5259,10 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5295,7 +5291,7 @@
         <v>137</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N30" t="s" s="2">
         <v>139</v>
@@ -5336,19 +5332,19 @@
         <v>81</v>
       </c>
       <c r="AB30" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="AC30" t="s" s="2">
         <v>275</v>
       </c>
-      <c r="AC30" t="s" s="2">
+      <c r="AD30" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AE30" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="AF30" t="s" s="2">
         <v>276</v>
-      </c>
-      <c r="AD30" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AE30" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="AF30" t="s" s="2">
-        <v>277</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>79</v>
@@ -5369,7 +5365,7 @@
         <v>81</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>81</v>
@@ -5380,10 +5376,10 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5406,19 +5402,19 @@
         <v>91</v>
       </c>
       <c r="K31" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="L31" t="s" s="2">
         <v>279</v>
       </c>
-      <c r="L31" t="s" s="2">
+      <c r="M31" t="s" s="2">
         <v>280</v>
       </c>
-      <c r="M31" t="s" s="2">
+      <c r="N31" t="s" s="2">
         <v>281</v>
       </c>
-      <c r="N31" t="s" s="2">
+      <c r="O31" t="s" s="2">
         <v>282</v>
-      </c>
-      <c r="O31" t="s" s="2">
-        <v>283</v>
       </c>
       <c r="P31" t="s" s="2">
         <v>81</v>
@@ -5467,7 +5463,7 @@
         <v>81</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>79</v>
@@ -5485,10 +5481,10 @@
         <v>81</v>
       </c>
       <c r="AL31" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="AM31" t="s" s="2">
         <v>285</v>
-      </c>
-      <c r="AM31" t="s" s="2">
-        <v>286</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>81</v>
@@ -5499,10 +5495,10 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5525,19 +5521,19 @@
         <v>91</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M32" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="N32" t="s" s="2">
         <v>289</v>
       </c>
-      <c r="N32" t="s" s="2">
+      <c r="O32" t="s" s="2">
         <v>290</v>
-      </c>
-      <c r="O32" t="s" s="2">
-        <v>291</v>
       </c>
       <c r="P32" t="s" s="2">
         <v>81</v>
@@ -5586,7 +5582,7 @@
         <v>81</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>79</v>
@@ -5604,10 +5600,10 @@
         <v>81</v>
       </c>
       <c r="AL32" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="AM32" t="s" s="2">
         <v>293</v>
-      </c>
-      <c r="AM32" t="s" s="2">
-        <v>294</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>81</v>
@@ -5618,10 +5614,10 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5644,17 +5640,17 @@
         <v>91</v>
       </c>
       <c r="K33" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="L33" t="s" s="2">
         <v>310</v>
       </c>
-      <c r="L33" t="s" s="2">
+      <c r="M33" t="s" s="2">
         <v>311</v>
-      </c>
-      <c r="M33" t="s" s="2">
-        <v>312</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="P33" t="s" s="2">
         <v>81</v>
@@ -5703,7 +5699,7 @@
         <v>81</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>79</v>
@@ -5721,10 +5717,10 @@
         <v>81</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>81</v>
@@ -5735,10 +5731,10 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5761,13 +5757,13 @@
         <v>91</v>
       </c>
       <c r="K34" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="L34" t="s" s="2">
         <v>316</v>
       </c>
-      <c r="L34" t="s" s="2">
+      <c r="M34" t="s" s="2">
         <v>317</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>318</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -5818,7 +5814,7 @@
         <v>81</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>90</v>
@@ -5833,31 +5829,31 @@
         <v>102</v>
       </c>
       <c r="AK34" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="AL34" t="s" s="2">
         <v>319</v>
       </c>
-      <c r="AL34" t="s" s="2">
+      <c r="AM34" t="s" s="2">
         <v>320</v>
       </c>
-      <c r="AM34" t="s" s="2">
+      <c r="AN34" t="s" s="2">
         <v>321</v>
       </c>
-      <c r="AN34" t="s" s="2">
+      <c r="AO34" t="s" s="2">
         <v>322</v>
-      </c>
-      <c r="AO34" t="s" s="2">
-        <v>323</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" t="s" s="2">
@@ -5876,13 +5872,13 @@
         <v>91</v>
       </c>
       <c r="K35" t="s" s="2">
+        <v>325</v>
+      </c>
+      <c r="L35" t="s" s="2">
         <v>326</v>
       </c>
-      <c r="L35" t="s" s="2">
+      <c r="M35" t="s" s="2">
         <v>327</v>
-      </c>
-      <c r="M35" t="s" s="2">
-        <v>328</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
@@ -5933,7 +5929,7 @@
         <v>81</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>79</v>
@@ -5948,31 +5944,31 @@
         <v>102</v>
       </c>
       <c r="AK35" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="AL35" t="s" s="2">
         <v>329</v>
       </c>
-      <c r="AL35" t="s" s="2">
+      <c r="AM35" t="s" s="2">
         <v>330</v>
       </c>
-      <c r="AM35" t="s" s="2">
+      <c r="AN35" t="s" s="2">
         <v>331</v>
       </c>
-      <c r="AN35" t="s" s="2">
+      <c r="AO35" t="s" s="2">
         <v>332</v>
-      </c>
-      <c r="AO35" t="s" s="2">
-        <v>333</v>
       </c>
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" t="s" s="2">
@@ -5991,13 +5987,13 @@
         <v>91</v>
       </c>
       <c r="K36" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="L36" t="s" s="2">
         <v>336</v>
       </c>
-      <c r="L36" t="s" s="2">
+      <c r="M36" t="s" s="2">
         <v>337</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>338</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -6048,7 +6044,7 @@
         <v>81</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>79</v>
@@ -6063,27 +6059,27 @@
         <v>102</v>
       </c>
       <c r="AK36" t="s" s="2">
+        <v>338</v>
+      </c>
+      <c r="AL36" t="s" s="2">
         <v>339</v>
       </c>
-      <c r="AL36" t="s" s="2">
+      <c r="AM36" t="s" s="2">
         <v>340</v>
       </c>
-      <c r="AM36" t="s" s="2">
+      <c r="AN36" t="s" s="2">
         <v>341</v>
       </c>
-      <c r="AN36" t="s" s="2">
+      <c r="AO36" t="s" s="2">
         <v>342</v>
-      </c>
-      <c r="AO36" t="s" s="2">
-        <v>343</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -6106,13 +6102,13 @@
         <v>91</v>
       </c>
       <c r="K37" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="L37" t="s" s="2">
         <v>345</v>
       </c>
-      <c r="L37" t="s" s="2">
+      <c r="M37" t="s" s="2">
         <v>346</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>347</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -6139,14 +6135,14 @@
         <v>81</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y37" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="Z37" t="s" s="2">
         <v>348</v>
       </c>
-      <c r="Z37" t="s" s="2">
-        <v>349</v>
-      </c>
       <c r="AA37" t="s" s="2">
         <v>81</v>
       </c>
@@ -6163,7 +6159,7 @@
         <v>81</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>79</v>
@@ -6184,25 +6180,25 @@
         <v>81</v>
       </c>
       <c r="AM37" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="AN37" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AO37" t="s" s="2">
         <v>350</v>
-      </c>
-      <c r="AN37" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AO37" t="s" s="2">
-        <v>351</v>
       </c>
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" t="s" s="2">
@@ -6221,13 +6217,13 @@
         <v>91</v>
       </c>
       <c r="K38" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="L38" t="s" s="2">
         <v>354</v>
       </c>
-      <c r="L38" t="s" s="2">
+      <c r="M38" t="s" s="2">
         <v>355</v>
-      </c>
-      <c r="M38" t="s" s="2">
-        <v>356</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
@@ -6278,7 +6274,7 @@
         <v>81</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>79</v>
@@ -6293,31 +6289,31 @@
         <v>102</v>
       </c>
       <c r="AK38" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="AL38" t="s" s="2">
         <v>357</v>
       </c>
-      <c r="AL38" t="s" s="2">
+      <c r="AM38" t="s" s="2">
         <v>358</v>
       </c>
-      <c r="AM38" t="s" s="2">
+      <c r="AN38" t="s" s="2">
         <v>359</v>
       </c>
-      <c r="AN38" t="s" s="2">
+      <c r="AO38" t="s" s="2">
         <v>360</v>
-      </c>
-      <c r="AO38" t="s" s="2">
-        <v>361</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" t="s" s="2">
@@ -6336,16 +6332,16 @@
         <v>91</v>
       </c>
       <c r="K39" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="L39" t="s" s="2">
         <v>364</v>
       </c>
-      <c r="L39" t="s" s="2">
+      <c r="M39" t="s" s="2">
         <v>365</v>
       </c>
-      <c r="M39" t="s" s="2">
+      <c r="N39" t="s" s="2">
         <v>366</v>
-      </c>
-      <c r="N39" t="s" s="2">
-        <v>367</v>
       </c>
       <c r="O39" s="2"/>
       <c r="P39" t="s" s="2">
@@ -6395,7 +6391,7 @@
         <v>81</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>79</v>
@@ -6410,31 +6406,31 @@
         <v>102</v>
       </c>
       <c r="AK39" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="AL39" t="s" s="2">
         <v>368</v>
       </c>
-      <c r="AL39" t="s" s="2">
+      <c r="AM39" t="s" s="2">
         <v>369</v>
       </c>
-      <c r="AM39" t="s" s="2">
+      <c r="AN39" t="s" s="2">
         <v>370</v>
       </c>
-      <c r="AN39" t="s" s="2">
+      <c r="AO39" t="s" s="2">
         <v>371</v>
-      </c>
-      <c r="AO39" t="s" s="2">
-        <v>372</v>
       </c>
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" t="s" s="2">
@@ -6453,16 +6449,16 @@
         <v>91</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L40" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="M40" t="s" s="2">
         <v>375</v>
       </c>
-      <c r="M40" t="s" s="2">
+      <c r="N40" t="s" s="2">
         <v>376</v>
-      </c>
-      <c r="N40" t="s" s="2">
-        <v>377</v>
       </c>
       <c r="O40" s="2"/>
       <c r="P40" t="s" s="2">
@@ -6488,14 +6484,14 @@
         <v>81</v>
       </c>
       <c r="X40" t="s" s="2">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y40" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="Z40" t="s" s="2">
         <v>378</v>
       </c>
-      <c r="Z40" t="s" s="2">
-        <v>379</v>
-      </c>
       <c r="AA40" t="s" s="2">
         <v>81</v>
       </c>
@@ -6512,7 +6508,7 @@
         <v>81</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>79</v>
@@ -6527,16 +6523,16 @@
         <v>102</v>
       </c>
       <c r="AK40" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="AL40" t="s" s="2">
         <v>380</v>
       </c>
-      <c r="AL40" t="s" s="2">
+      <c r="AM40" t="s" s="2">
         <v>381</v>
       </c>
-      <c r="AM40" t="s" s="2">
+      <c r="AN40" t="s" s="2">
         <v>382</v>
-      </c>
-      <c r="AN40" t="s" s="2">
-        <v>383</v>
       </c>
       <c r="AO40" t="s" s="2">
         <v>81</v>
@@ -6544,14 +6540,14 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" t="s" s="2">
@@ -6570,16 +6566,16 @@
         <v>91</v>
       </c>
       <c r="K41" t="s" s="2">
+        <v>385</v>
+      </c>
+      <c r="L41" t="s" s="2">
         <v>386</v>
       </c>
-      <c r="L41" t="s" s="2">
+      <c r="M41" t="s" s="2">
         <v>387</v>
       </c>
-      <c r="M41" t="s" s="2">
+      <c r="N41" t="s" s="2">
         <v>388</v>
-      </c>
-      <c r="N41" t="s" s="2">
-        <v>389</v>
       </c>
       <c r="O41" s="2"/>
       <c r="P41" t="s" s="2">
@@ -6629,7 +6625,7 @@
         <v>81</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>79</v>
@@ -6644,16 +6640,16 @@
         <v>102</v>
       </c>
       <c r="AK41" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="AL41" t="s" s="2">
         <v>390</v>
       </c>
-      <c r="AL41" t="s" s="2">
+      <c r="AM41" t="s" s="2">
         <v>391</v>
       </c>
-      <c r="AM41" t="s" s="2">
-        <v>392</v>
-      </c>
       <c r="AN41" t="s" s="2">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AO41" t="s" s="2">
         <v>81</v>
@@ -6661,10 +6657,10 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6687,13 +6683,13 @@
         <v>91</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L42" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="M42" t="s" s="2">
         <v>394</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>395</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
@@ -6720,14 +6716,14 @@
         <v>81</v>
       </c>
       <c r="X42" t="s" s="2">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y42" t="s" s="2">
+        <v>395</v>
+      </c>
+      <c r="Z42" t="s" s="2">
         <v>396</v>
       </c>
-      <c r="Z42" t="s" s="2">
-        <v>397</v>
-      </c>
       <c r="AA42" t="s" s="2">
         <v>81</v>
       </c>
@@ -6744,7 +6740,7 @@
         <v>81</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>79</v>
@@ -6765,10 +6761,10 @@
         <v>81</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="AN42" t="s" s="2">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AO42" t="s" s="2">
         <v>81</v>
@@ -6776,10 +6772,10 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6802,13 +6798,13 @@
         <v>91</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="L43" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="M43" t="s" s="2">
         <v>400</v>
-      </c>
-      <c r="L43" t="s" s="2">
-        <v>394</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>401</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
@@ -6859,7 +6855,7 @@
         <v>81</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>79</v>
@@ -6880,10 +6876,10 @@
         <v>81</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AN43" t="s" s="2">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AO43" t="s" s="2">
         <v>81</v>
@@ -6891,10 +6887,10 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6917,16 +6913,16 @@
         <v>91</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L44" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="M44" t="s" s="2">
         <v>404</v>
       </c>
-      <c r="M44" t="s" s="2">
+      <c r="N44" t="s" s="2">
         <v>405</v>
-      </c>
-      <c r="N44" t="s" s="2">
-        <v>406</v>
       </c>
       <c r="O44" s="2"/>
       <c r="P44" t="s" s="2">
@@ -6952,11 +6948,11 @@
         <v>81</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Y44" s="2"/>
       <c r="Z44" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AA44" t="s" s="2">
         <v>81</v>
@@ -6974,7 +6970,7 @@
         <v>81</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>79</v>
@@ -6989,16 +6985,16 @@
         <v>102</v>
       </c>
       <c r="AK44" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="AL44" t="s" s="2">
         <v>408</v>
       </c>
-      <c r="AL44" t="s" s="2">
+      <c r="AM44" t="s" s="2">
         <v>409</v>
       </c>
-      <c r="AM44" t="s" s="2">
+      <c r="AN44" t="s" s="2">
         <v>410</v>
-      </c>
-      <c r="AN44" t="s" s="2">
-        <v>411</v>
       </c>
       <c r="AO44" t="s" s="2">
         <v>81</v>
@@ -7006,10 +7002,10 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -7032,16 +7028,16 @@
         <v>91</v>
       </c>
       <c r="K45" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="L45" t="s" s="2">
         <v>413</v>
       </c>
-      <c r="L45" t="s" s="2">
+      <c r="M45" t="s" s="2">
         <v>414</v>
       </c>
-      <c r="M45" t="s" s="2">
+      <c r="N45" t="s" s="2">
         <v>415</v>
-      </c>
-      <c r="N45" t="s" s="2">
-        <v>416</v>
       </c>
       <c r="O45" s="2"/>
       <c r="P45" t="s" s="2">
@@ -7091,7 +7087,7 @@
         <v>81</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>79</v>
@@ -7106,16 +7102,16 @@
         <v>102</v>
       </c>
       <c r="AK45" t="s" s="2">
+        <v>416</v>
+      </c>
+      <c r="AL45" t="s" s="2">
         <v>417</v>
       </c>
-      <c r="AL45" t="s" s="2">
+      <c r="AM45" t="s" s="2">
         <v>418</v>
       </c>
-      <c r="AM45" t="s" s="2">
-        <v>419</v>
-      </c>
       <c r="AN45" t="s" s="2">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AO45" t="s" s="2">
         <v>81</v>
@@ -7123,10 +7119,10 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -7149,13 +7145,13 @@
         <v>81</v>
       </c>
       <c r="K46" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="L46" t="s" s="2">
         <v>421</v>
       </c>
-      <c r="L46" t="s" s="2">
+      <c r="M46" t="s" s="2">
         <v>422</v>
-      </c>
-      <c r="M46" t="s" s="2">
-        <v>423</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
@@ -7206,7 +7202,7 @@
         <v>81</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>79</v>
@@ -7221,13 +7217,13 @@
         <v>102</v>
       </c>
       <c r="AK46" t="s" s="2">
+        <v>423</v>
+      </c>
+      <c r="AL46" t="s" s="2">
         <v>424</v>
       </c>
-      <c r="AL46" t="s" s="2">
+      <c r="AM46" t="s" s="2">
         <v>425</v>
-      </c>
-      <c r="AM46" t="s" s="2">
-        <v>426</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>81</v>
@@ -7238,14 +7234,14 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" t="s" s="2">
@@ -7264,16 +7260,16 @@
         <v>81</v>
       </c>
       <c r="K47" t="s" s="2">
+        <v>428</v>
+      </c>
+      <c r="L47" t="s" s="2">
         <v>429</v>
       </c>
-      <c r="L47" t="s" s="2">
+      <c r="M47" t="s" s="2">
         <v>430</v>
       </c>
-      <c r="M47" t="s" s="2">
+      <c r="N47" t="s" s="2">
         <v>431</v>
-      </c>
-      <c r="N47" t="s" s="2">
-        <v>432</v>
       </c>
       <c r="O47" s="2"/>
       <c r="P47" t="s" s="2">
@@ -7323,7 +7319,7 @@
         <v>81</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>79</v>
@@ -7338,13 +7334,13 @@
         <v>102</v>
       </c>
       <c r="AK47" t="s" s="2">
+        <v>432</v>
+      </c>
+      <c r="AL47" t="s" s="2">
         <v>433</v>
       </c>
-      <c r="AL47" t="s" s="2">
+      <c r="AM47" t="s" s="2">
         <v>434</v>
-      </c>
-      <c r="AM47" t="s" s="2">
-        <v>435</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>81</v>
@@ -7355,10 +7351,10 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7381,16 +7377,16 @@
         <v>91</v>
       </c>
       <c r="K48" t="s" s="2">
+        <v>436</v>
+      </c>
+      <c r="L48" t="s" s="2">
         <v>437</v>
       </c>
-      <c r="L48" t="s" s="2">
+      <c r="M48" t="s" s="2">
         <v>438</v>
       </c>
-      <c r="M48" t="s" s="2">
+      <c r="N48" t="s" s="2">
         <v>439</v>
-      </c>
-      <c r="N48" t="s" s="2">
-        <v>440</v>
       </c>
       <c r="O48" s="2"/>
       <c r="P48" t="s" s="2">
@@ -7440,7 +7436,7 @@
         <v>81</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>79</v>
@@ -7458,10 +7454,10 @@
         <v>81</v>
       </c>
       <c r="AL48" t="s" s="2">
+        <v>440</v>
+      </c>
+      <c r="AM48" t="s" s="2">
         <v>441</v>
-      </c>
-      <c r="AM48" t="s" s="2">
-        <v>442</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>81</v>
@@ -7472,14 +7468,14 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" t="s" s="2">
@@ -7498,19 +7494,19 @@
         <v>91</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L49" t="s" s="2">
+        <v>444</v>
+      </c>
+      <c r="M49" t="s" s="2">
         <v>445</v>
       </c>
-      <c r="M49" t="s" s="2">
+      <c r="N49" t="s" s="2">
         <v>446</v>
       </c>
-      <c r="N49" t="s" s="2">
+      <c r="O49" t="s" s="2">
         <v>447</v>
-      </c>
-      <c r="O49" t="s" s="2">
-        <v>448</v>
       </c>
       <c r="P49" t="s" s="2">
         <v>81</v>
@@ -7535,14 +7531,14 @@
         <v>81</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y49" t="s" s="2">
+        <v>448</v>
+      </c>
+      <c r="Z49" t="s" s="2">
         <v>449</v>
       </c>
-      <c r="Z49" t="s" s="2">
-        <v>450</v>
-      </c>
       <c r="AA49" t="s" s="2">
         <v>81</v>
       </c>
@@ -7559,7 +7555,7 @@
         <v>81</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>79</v>
@@ -7577,24 +7573,24 @@
         <v>81</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="AM49" t="s" s="2">
+        <v>450</v>
+      </c>
+      <c r="AN49" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AO49" t="s" s="2">
         <v>451</v>
-      </c>
-      <c r="AN49" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AO49" t="s" s="2">
-        <v>452</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -7617,13 +7613,13 @@
         <v>81</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="L50" t="s" s="2">
         <v>50</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
@@ -7674,7 +7670,7 @@
         <v>81</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>79</v>
@@ -7689,27 +7685,27 @@
         <v>102</v>
       </c>
       <c r="AK50" t="s" s="2">
+        <v>455</v>
+      </c>
+      <c r="AL50" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="AM50" t="s" s="2">
         <v>456</v>
       </c>
-      <c r="AL50" t="s" s="2">
-        <v>303</v>
-      </c>
-      <c r="AM50" t="s" s="2">
+      <c r="AN50" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AO50" t="s" s="2">
         <v>457</v>
-      </c>
-      <c r="AN50" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AO50" t="s" s="2">
-        <v>458</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7732,13 +7728,13 @@
         <v>91</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L51" t="s" s="2">
+        <v>459</v>
+      </c>
+      <c r="M51" t="s" s="2">
         <v>460</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>461</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
@@ -7789,7 +7785,7 @@
         <v>81</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>79</v>
@@ -7807,10 +7803,10 @@
         <v>81</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>81</v>
@@ -7821,10 +7817,10 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -7847,16 +7843,16 @@
         <v>81</v>
       </c>
       <c r="K52" t="s" s="2">
+        <v>463</v>
+      </c>
+      <c r="L52" t="s" s="2">
         <v>464</v>
       </c>
-      <c r="L52" t="s" s="2">
+      <c r="M52" t="s" s="2">
         <v>465</v>
       </c>
-      <c r="M52" t="s" s="2">
+      <c r="N52" t="s" s="2">
         <v>466</v>
-      </c>
-      <c r="N52" t="s" s="2">
-        <v>467</v>
       </c>
       <c r="O52" s="2"/>
       <c r="P52" t="s" s="2">
@@ -7906,7 +7902,7 @@
         <v>81</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>79</v>
@@ -7921,13 +7917,13 @@
         <v>102</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="AL52" t="s" s="2">
         <v>133</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>81</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ Healthedata1/test-stuff@c23c7ffe5bcf639fcfe60f04c7345353f9136da1 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-pmo-servicerequest.xlsx
+++ b/StructureDefinition-us-core-pmo-servicerequest.xlsx
@@ -375,7 +375,7 @@
     <t>A human language.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/languages</t>
+    <t>http://hl7.org/fhir/ValueSet/languages|4.0.1</t>
   </si>
   <si>
     <t>Resource.language</t>
@@ -510,7 +510,7 @@
     <t>ServiceRequest.instantiatesCanonical</t>
   </si>
   <si>
-    <t xml:space="preserve">canonical(ActivityDefinition|PlanDefinition)
+    <t xml:space="preserve">canonical(ActivityDefinition|4.0.1|PlanDefinition|4.0.1)
 </t>
   </si>
   <si>
@@ -554,7 +554,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(CarePlan|ServiceRequest|MedicationRequest)
+    <t xml:space="preserve">Reference(CarePlan|4.0.1|ServiceRequest|4.0.1|MedicationRequest|4.0.1)
 </t>
   </si>
   <si>
@@ -580,7 +580,7 @@
 priorrenewed order</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(ServiceRequest)
+    <t xml:space="preserve">Reference(ServiceRequest|4.0.1)
 </t>
   </si>
   <si>
@@ -715,7 +715,7 @@
     <t>Classification of the requested service.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/servicerequest-category</t>
+    <t>http://hl7.org/fhir/ValueSet/servicerequest-category|4.0.1</t>
   </si>
   <si>
     <t xml:space="preserve">value:$this}
@@ -951,7 +951,7 @@
     <t>Codified order entry details which are based on order context.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/servicerequest-orderdetail</t>
+    <t>http://hl7.org/fhir/ValueSet/servicerequest-orderdetail|4.0.1</t>
   </si>
   <si>
     <t xml:space="preserve">prr-1
@@ -1103,7 +1103,7 @@
     <t>A coded concept identifying the pre-condition that should hold prior to performing a procedure.  For example "pain", "on flare-up", etc.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/medication-as-needed-reason</t>
+    <t>http://hl7.org/fhir/ValueSet/medication-as-needed-reason|4.0.1</t>
   </si>
   <si>
     <t>boolean: precondition.negationInd (inversed - so negationInd = true means asNeeded=false CodeableConcept: precondition.observationEventCriterion[code="Assertion"].value</t>
@@ -1198,7 +1198,7 @@
     <t>Indicates specific responsibility of an individual within the care team, such as "Primary physician", "Team coordinator", "Caregiver", etc.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/participant-role</t>
+    <t>http://hl7.org/fhir/ValueSet/participant-role|4.0.1</t>
   </si>
   <si>
     <t>Request.performerType</t>
@@ -1220,7 +1220,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Practitioner|PractitionerRole|Organization|CareTeam|HealthcareService|Patient|Device|RelatedPerson)
+    <t xml:space="preserve">Reference(Practitioner|4.0.1|PractitionerRole|4.0.1|Organization|4.0.1|CareTeam|4.0.1|HealthcareService|4.0.1|Patient|4.0.1|Device|4.0.1|RelatedPerson|4.0.1)
 </t>
   </si>
   <si>
@@ -1263,7 +1263,7 @@
     <t>ServiceRequest.locationReference</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Location)
+    <t xml:space="preserve">Reference(Location|4.0.1)
 </t>
   </si>
   <si>
@@ -1328,7 +1328,7 @@
     <t>ServiceRequest.insurance</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Coverage|ClaimResponse)
+    <t xml:space="preserve">Reference(Coverage|4.0.1|ClaimResponse|4.0.1)
 </t>
   </si>
   <si>
@@ -1354,7 +1354,7 @@
 AOE</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Resource)
+    <t xml:space="preserve">Reference(Resource|4.0.1)
 </t>
   </si>
   <si>
@@ -1379,7 +1379,7 @@
     <t>ServiceRequest.specimen</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Specimen)
+    <t xml:space="preserve">Reference(Specimen|4.0.1)
 </t>
   </si>
   <si>
@@ -1420,7 +1420,7 @@
     <t>Codes describing anatomical locations. May include laterality.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/body-site</t>
+    <t>http://hl7.org/fhir/ValueSet/body-site|4.0.1</t>
   </si>
   <si>
     <t>targetSiteCode</t>
@@ -1463,7 +1463,7 @@
     <t>ServiceRequest.relevantHistory</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Provenance)
+    <t xml:space="preserve">Reference(Provenance|4.0.1)
 </t>
   </si>
   <si>

</xml_diff>